<commit_message>
Commited qua 11 nov 2020 11:25:54 -03 @ X580VD
</commit_message>
<xml_diff>
--- a/Calendário de Entregas.xlsx
+++ b/Calendário de Entregas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>Semana</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>**</t>
+  </si>
+  <si>
+    <t>EM PROGRESSO</t>
   </si>
   <si>
     <t>UNIDADE 13 - Carreira e Conclusão</t>
@@ -1188,14 +1191,14 @@
         <v>60</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" ht="30.0" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="11"/>
       <c r="C36" s="35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>

</xml_diff>

<commit_message>
Commited qua 11 nov 2020 11:39:20 -03 @ X580VD
</commit_message>
<xml_diff>
--- a/Calendário de Entregas.xlsx
+++ b/Calendário de Entregas.xlsx
@@ -65,6 +65,9 @@
     </r>
   </si>
   <si>
+    <t>PENDENTE</t>
+  </si>
+  <si>
     <t>LEGENDA</t>
   </si>
   <si>
@@ -80,9 +83,6 @@
       </rPr>
       <t>*</t>
     </r>
-  </si>
-  <si>
-    <t>PENDENTE</t>
   </si>
   <si>
     <t>ATIVIDADE DA PLATAFORMA</t>
@@ -705,7 +705,7 @@
       </c>
       <c r="I2" s="5">
         <f>SUMIF(F:F,"COMPLETO",E:E)</f>
-        <v>1020</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" ht="30.0" customHeight="1">
@@ -768,13 +768,13 @@
         <v>80.0</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="19"/>
@@ -784,13 +784,13 @@
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
       <c r="D7" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="8">
         <v>80.0</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>18</v>
@@ -812,7 +812,7 @@
         <v>80.0</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>21</v>
@@ -834,7 +834,7 @@
         <v>60.0</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H9" s="21" t="s">
         <v>24</v>
@@ -888,7 +888,7 @@
         <v>60.0</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="24"/>
@@ -940,7 +940,7 @@
         <v>60.0</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="K15" s="16"/>
       <c r="L15" s="31"/>
@@ -1001,7 +1001,7 @@
         <v>60.0</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H19" s="32"/>
     </row>
@@ -1074,7 +1074,7 @@
         <v>80.0</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26">
@@ -1123,7 +1123,7 @@
         <v>100.0</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -1144,7 +1144,7 @@
         <v>60.0</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32">

</xml_diff>

<commit_message>
Commited qua 11 nov 2020 11:48:56 -03 @ X580VD
</commit_message>
<xml_diff>
--- a/Calendário de Entregas.xlsx
+++ b/Calendário de Entregas.xlsx
@@ -705,7 +705,7 @@
       </c>
       <c r="I2" s="5">
         <f>SUMIF(F:F,"COMPLETO",E:E)</f>
-        <v>1000</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="3" ht="30.0" customHeight="1">
@@ -1144,7 +1144,7 @@
         <v>60.0</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">

</xml_diff>